<commit_message>
fixed a dang page
</commit_message>
<xml_diff>
--- a/docs/7-30-2025 BBB Frontend Review Comments.xlsx
+++ b/docs/7-30-2025 BBB Frontend Review Comments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\busybeeboard\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E38421-7FE5-48BB-BB2B-5A995CFB584B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1866811-9CD1-47B0-B0ED-FBBE0DEF99C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7E69E474-E2A0-4391-AAE9-29C85B6E0562}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>about-us</t>
   </si>
@@ -548,7 +548,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +653,9 @@
         <v>17</v>
       </c>
       <c r="C8" s="8"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">

</xml_diff>